<commit_message>
Item Summary compeleted according to requirements
</commit_message>
<xml_diff>
--- a/ItemSummary.xlsx
+++ b/ItemSummary.xlsx
@@ -397,17 +397,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C26"/>
+  <dimension ref="A1:C17"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetData>
     <row r="1">
       <c r="A1" t="str">
-        <v>Item ▲▼</v>
+        <v>Item</v>
       </c>
       <c r="B1" t="str">
-        <v>Quantity ▲▼</v>
+        <v>Quantity</v>
       </c>
       <c r="C1" t="str">
         <v>Revenue ▼</v>
@@ -415,244 +415,160 @@
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>Burgers</v>
+        <v>Lassi</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="str">
-        <v>Chicken Cheese Burger</v>
+        <v>Mango Lassi</v>
       </c>
       <c r="B3">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C3" t="str">
-        <v>₹360.00</v>
+        <v>₹480.00</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="str">
-        <v>Chicken Borgir</v>
+        <v>Butterscotch Lassi</v>
       </c>
       <c r="B4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C4" t="str">
-        <v>₹120.00</v>
+        <v>₹60.00</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="str">
-        <v>Lassi</v>
+        <v>Strawberry Lassi</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5" t="str">
+        <v>₹40.00</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="str">
-        <v>Mango Lassi</v>
-      </c>
-      <c r="B6">
-        <v>3</v>
-      </c>
-      <c r="C6" t="str">
-        <v>₹180.00</v>
+        <v>Burgers</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="str">
-        <v>Strawberry Lassi</v>
+        <v>Chicken Cheese Burger</v>
       </c>
       <c r="B7">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C7" t="str">
-        <v>₹40.00</v>
+        <v>₹180.00</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="str">
-        <v>Wraps</v>
+        <v>Chicken Burger</v>
+      </c>
+      <c r="B8">
+        <v>2</v>
+      </c>
+      <c r="C8" t="str">
+        <v>₹120.00</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="str">
-        <v>Chicken Wrap</v>
-      </c>
-      <c r="B9">
-        <v>3</v>
-      </c>
-      <c r="C9" t="str">
-        <v>₹180.00</v>
+        <v>Pops</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="str">
-        <v>Veg Wrap</v>
+        <v>Veg Cheese Pops</v>
       </c>
       <c r="B10">
         <v>1</v>
       </c>
       <c r="C10" t="str">
-        <v>₹50.00</v>
+        <v>₹70.00</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="str">
-        <v>Cold Coffee</v>
+        <v>Chicken Cheese Pops</v>
+      </c>
+      <c r="B11">
+        <v>1</v>
+      </c>
+      <c r="C11" t="str">
+        <v>₹70.00</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="str">
-        <v>Belgian Coffee</v>
-      </c>
-      <c r="B12">
-        <v>3</v>
-      </c>
-      <c r="C12" t="str">
-        <v>₹120.00</v>
+        <v>Wraps</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="str">
-        <v>8PM Coffee</v>
+        <v>Chicken Wrap</v>
       </c>
       <c r="B13">
         <v>1</v>
       </c>
       <c r="C13" t="str">
-        <v>₹40.00</v>
+        <v>₹60.00</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="str">
-        <v>Coffee Italia</v>
-      </c>
-      <c r="B14">
-        <v>1</v>
-      </c>
-      <c r="C14" t="str">
-        <v>₹40.00</v>
+        <v>Milkshakes</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="str">
-        <v>Hard Rock Coffee</v>
+        <v>Oreo Shake</v>
       </c>
       <c r="B15">
         <v>1</v>
       </c>
       <c r="C15" t="str">
-        <v>₹40.00</v>
+        <v>₹50.00</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="str">
-        <v>Juices</v>
+        <v>Banana Shake</v>
+      </c>
+      <c r="B16">
+        <v>1</v>
+      </c>
+      <c r="C16" t="str">
+        <v>₹50.00</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="str">
-        <v>Weed</v>
+        <v>Vanilla Shake</v>
       </c>
       <c r="B17">
         <v>1</v>
       </c>
       <c r="C17" t="str">
-        <v>₹100.00</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" t="str">
-        <v>Lime Juice</v>
-      </c>
-      <c r="B18">
-        <v>3</v>
-      </c>
-      <c r="C18" t="str">
-        <v>₹60.00</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="str">
-        <v>Mint Lime</v>
-      </c>
-      <c r="B19">
-        <v>1</v>
-      </c>
-      <c r="C19" t="str">
-        <v>₹30.00</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" t="str">
-        <v>Pops</v>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" t="str">
-        <v>Veg Cheese Pops</v>
-      </c>
-      <c r="B21">
-        <v>1</v>
-      </c>
-      <c r="C21" t="str">
-        <v>₹70.00</v>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" t="str">
-        <v>Milkshakes</v>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" t="str">
-        <v>Oreo Shake</v>
-      </c>
-      <c r="B23">
-        <v>1</v>
-      </c>
-      <c r="C23" t="str">
-        <v>₹50.00</v>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" t="str">
-        <v>Vanilla Shake</v>
-      </c>
-      <c r="B24">
-        <v>1</v>
-      </c>
-      <c r="C24" t="str">
         <v>₹40.00</v>
       </c>
     </row>
-    <row r="25">
-      <c r="A25" t="str">
-        <v>French Fries</v>
-      </c>
-    </row>
-    <row r="26">
-      <c r="A26" t="str">
-        <v>Peri Peri Fries</v>
-      </c>
-      <c r="B26">
-        <v>1</v>
-      </c>
-      <c r="C26" t="str">
-        <v>₹20.00</v>
-      </c>
-    </row>
   </sheetData>
-  <mergeCells count="8">
+  <mergeCells count="5">
     <mergeCell ref="A2:C2"/>
-    <mergeCell ref="A5:C5"/>
-    <mergeCell ref="A8:C8"/>
-    <mergeCell ref="A11:C11"/>
-    <mergeCell ref="A16:C16"/>
-    <mergeCell ref="A20:C20"/>
-    <mergeCell ref="A22:C22"/>
-    <mergeCell ref="A25:C25"/>
+    <mergeCell ref="A6:C6"/>
+    <mergeCell ref="A9:C9"/>
+    <mergeCell ref="A12:C12"/>
+    <mergeCell ref="A14:C14"/>
   </mergeCells>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:C26"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:C17"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>